<commit_message>
updated the #defines for nextion display
</commit_message>
<xml_diff>
--- a/hardware/rev 4/Aries parts list rev 4.xlsx
+++ b/hardware/rev 4/Aries parts list rev 4.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{FE589F85-F430-46E0-9844-581DB2745167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0AA7B1C5-2C8A-4D3A-8170-CCE7B2AF8D3C}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{FE589F85-F430-46E0-9844-581DB2745167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BE5956AD-C4A4-4CBC-896F-B0B11FDAEC3E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="189">
   <si>
     <t>RL1-RL17</t>
   </si>
@@ -264,18 +264,9 @@
     <t>2K7 0603</t>
   </si>
   <si>
-    <t>RL18</t>
-  </si>
-  <si>
-    <t>RL19-21</t>
-  </si>
-  <si>
     <t>Omron G6A-274P</t>
   </si>
   <si>
-    <t>3-1462039-8</t>
-  </si>
-  <si>
     <t>L14-15</t>
   </si>
   <si>
@@ -285,9 +276,6 @@
     <t>0805 size, 100 ohm@10MHz</t>
   </si>
   <si>
-    <t>D22, D27,D32, D50</t>
-  </si>
-  <si>
     <t>red 0805</t>
   </si>
   <si>
@@ -531,9 +519,6 @@
     <t>The VSWR bridge is now a binocular core using a BN-61-202 core</t>
   </si>
   <si>
-    <t>secondary: 10T 26SWG wound around the sides of the core</t>
-  </si>
-  <si>
     <t>BNC rt angle</t>
   </si>
   <si>
@@ -594,9 +579,10 @@
     <t>616-3084</t>
   </si>
   <si>
-    <t>RS 422-7079
-DigiKey PB2078-ND
-Mouser 655-3-1462039-8</t>
+    <t>RL18-21</t>
+  </si>
+  <si>
+    <t>secondary: 10T 26 SWG wound around the sides of the core</t>
   </si>
 </sst>
 </file>
@@ -1087,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,7 +1086,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>35</v>
@@ -1211,16 +1197,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -1297,16 +1283,16 @@
         <v>17</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -1315,13 +1301,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -1331,17 +1317,17 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1365,7 +1351,7 @@
         <v>52</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>23</v>
@@ -1387,7 +1373,7 @@
         <v>23</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1435,7 +1421,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -1483,7 +1469,7 @@
         <v>23</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1499,7 +1485,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1541,7 +1527,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>23</v>
@@ -1557,7 +1543,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>23</v>
@@ -1573,7 +1559,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>23</v>
@@ -1589,17 +1575,17 @@
         <v>2</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1607,16 +1593,16 @@
         <v>6</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F31" s="5"/>
     </row>
@@ -1631,7 +1617,7 @@
         <v>39</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -1641,13 +1627,13 @@
         <v>7</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -1663,7 +1649,7 @@
         <v>39</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -1679,7 +1665,7 @@
         <v>39</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -1689,18 +1675,18 @@
         <v>2</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1714,12 +1700,12 @@
         <v>39</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1727,13 +1713,13 @@
         <v>17</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -1743,16 +1729,16 @@
         <v>1</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F39" s="5"/>
     </row>
@@ -1761,13 +1747,13 @@
         <v>2</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -1777,13 +1763,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -1793,13 +1779,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -1827,13 +1813,13 @@
         <v>2</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>65</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -1843,17 +1829,17 @@
         <v>2</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1861,16 +1847,16 @@
         <v>2</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D46" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>191</v>
       </c>
       <c r="F46" s="5"/>
     </row>
@@ -1879,16 +1865,16 @@
         <v>1</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F47" s="5"/>
     </row>
@@ -1897,13 +1883,13 @@
         <v>1</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -1913,13 +1899,13 @@
         <v>1</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -1929,17 +1915,17 @@
         <v>1</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1947,143 +1933,143 @@
         <v>2</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C57" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C58" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C59" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="C60" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C61" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C62" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C65" s="7" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2095,10 +2081,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2112,7 +2098,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>35</v>
@@ -2133,13 +2119,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2165,7 +2151,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>65</v>
@@ -2183,13 +2169,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>65</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2199,10 +2185,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -2220,7 +2206,7 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -2304,110 +2290,93 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>82</v>
+        <v>187</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>192</v>
+        <v>129</v>
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>3</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>83</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B14" s="6"/>
       <c r="C14" s="5" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>133</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>4</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>128</v>
+      </c>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>132</v>
-      </c>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
@@ -2445,9 +2414,6 @@
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>